<commit_message>
Changed the date formatting method to remove leading zeroes
</commit_message>
<xml_diff>
--- a/Warehouse_Ship_Days.xlsx
+++ b/Warehouse_Ship_Days.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1ad0f44da62cdc4c/Documents/ARN-Invoice_Submissions/ARN-Invoice_Submissions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming Projects\ASN_Sub_Automator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{75F57BB6-0627-405A-9409-1032204A7D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC2B8D06-B0B1-4259-86F2-A6DEE4AC81C6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8481F6-BB59-4584-9521-D7A7DA135C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6294DBFF-D57F-4B78-B461-50A917CE3F08}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="15800" xr2:uid="{6294DBFF-D57F-4B78-B461-50A917CE3F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="325">
   <si>
     <t>DFW6</t>
   </si>
@@ -993,19 +993,43 @@
   </si>
   <si>
     <t>PPO4</t>
+  </si>
+  <si>
+    <t>ABQ2</t>
+  </si>
+  <si>
+    <t>ABQ2 - LOS LUNAS, NM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ABS4 - Las Vegas, NV</t>
+  </si>
+  <si>
+    <t>LAN2 - Lansing, MI</t>
+  </si>
+  <si>
+    <t>TMB8 - Homestead, FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPO4 - Crown Point, IN </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF232F3E"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1028,8 +1052,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,8 +1075,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B6E22FBF-C66A-4900-86C7-48A68D156AD8}" name="Table1" displayName="Table1" ref="A1:C163" totalsRowShown="0">
   <autoFilter ref="A1:C163" xr:uid="{B6E22FBF-C66A-4900-86C7-48A68D156AD8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C162">
-    <sortCondition ref="A1:A162"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C163">
+    <sortCondition ref="A1:A163"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{4D54B485-E84A-4D0C-98D3-AF6F63F95805}" name="Warehouse Code"/>
@@ -1381,15 +1406,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4662F2-FD79-40A4-9787-FD9B0FF81454}">
   <dimension ref="A1:C163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1426,30 +1451,33 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>314</v>
+      <c r="A4" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B4" t="s">
+        <v>320</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>314</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>321</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>240</v>
+        <v>88</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1457,10 +1485,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>239</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>240</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1468,43 +1496,43 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>241</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>242</v>
+        <v>90</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>241</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>242</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -1512,43 +1540,43 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>243</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>94</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>243</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>244</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>219</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>220</v>
+        <v>96</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -1556,21 +1584,21 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>221</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>222</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>97</v>
       </c>
       <c r="B17" t="s">
-        <v>246</v>
+        <v>98</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -1578,10 +1606,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>245</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>246</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -1589,10 +1617,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -1600,32 +1628,32 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>247</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>248</v>
+        <v>25</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>247</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>248</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1633,10 +1661,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -1644,10 +1672,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>249</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>250</v>
+        <v>106</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -1655,10 +1683,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>249</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>250</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1666,10 +1694,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1677,10 +1705,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -1688,10 +1716,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -1699,10 +1727,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1710,21 +1738,21 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>315</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>251</v>
+        <v>315</v>
       </c>
       <c r="B31" t="s">
-        <v>252</v>
+        <v>26</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1732,21 +1760,21 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B32" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>253</v>
       </c>
       <c r="B33" t="s">
-        <v>118</v>
+        <v>254</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -1754,10 +1782,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B34" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -1765,32 +1793,32 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B37" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C37">
         <v>3</v>
@@ -1798,10 +1826,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>257</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>258</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -1809,32 +1837,32 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1842,10 +1870,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1853,10 +1881,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1864,54 +1892,54 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>259</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>260</v>
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="B45" t="s">
-        <v>224</v>
+        <v>260</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>123</v>
+        <v>223</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>224</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>261</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>262</v>
+        <v>30</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -1919,21 +1947,21 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B49" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B50" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1941,10 +1969,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>125</v>
+        <v>265</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>266</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -1952,10 +1980,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>309</v>
+        <v>125</v>
       </c>
       <c r="B52" t="s">
-        <v>310</v>
+        <v>126</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -1963,10 +1991,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="B53" t="s">
-        <v>268</v>
+        <v>310</v>
       </c>
       <c r="C53">
         <v>3</v>
@@ -1974,21 +2002,21 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>267</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>268</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>269</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>270</v>
+        <v>11</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1996,10 +2024,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>269</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>270</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -2007,43 +2035,43 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>271</v>
+        <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>272</v>
+        <v>32</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>33</v>
+        <v>271</v>
       </c>
       <c r="B59" t="s">
-        <v>34</v>
+        <v>272</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C60">
         <v>2</v>
@@ -2051,21 +2079,21 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="B61" t="s">
-        <v>128</v>
+        <v>36</v>
       </c>
       <c r="C61">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B62" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C62">
         <v>3</v>
@@ -2073,10 +2101,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B63" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C63">
         <v>3</v>
@@ -2084,10 +2112,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B64" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C64">
         <v>3</v>
@@ -2095,10 +2123,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C65">
         <v>3</v>
@@ -2109,7 +2137,7 @@
         <v>135</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C66">
         <v>3</v>
@@ -2117,40 +2145,43 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>273</v>
+        <v>135</v>
       </c>
       <c r="B67" t="s">
-        <v>274</v>
+        <v>137</v>
       </c>
       <c r="C67">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>273</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>274</v>
       </c>
       <c r="C68">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="B69" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>313</v>
+        <v>37</v>
+      </c>
+      <c r="B70" t="s">
+        <v>38</v>
       </c>
       <c r="C70">
         <v>2</v>
@@ -2158,21 +2189,21 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>225</v>
+        <v>313</v>
       </c>
       <c r="B71" t="s">
-        <v>226</v>
+        <v>322</v>
       </c>
       <c r="C71">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C72">
         <v>4</v>
@@ -2180,43 +2211,43 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>311</v>
+        <v>227</v>
       </c>
       <c r="B73" t="s">
-        <v>312</v>
+        <v>228</v>
       </c>
       <c r="C73">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>311</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
+        <v>312</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="B75" t="s">
-        <v>141</v>
+        <v>40</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -2224,10 +2255,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>275</v>
+        <v>142</v>
       </c>
       <c r="B77" t="s">
-        <v>276</v>
+        <v>143</v>
       </c>
       <c r="C77">
         <v>3</v>
@@ -2235,10 +2266,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B78" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -2246,54 +2277,54 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
       <c r="B79" t="s">
-        <v>15</v>
+        <v>278</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>279</v>
+        <v>14</v>
       </c>
       <c r="B80" t="s">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="C80">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B81" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>144</v>
+        <v>281</v>
       </c>
       <c r="B82" t="s">
-        <v>145</v>
+        <v>282</v>
       </c>
       <c r="C82">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B83" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -2301,10 +2332,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>283</v>
+        <v>146</v>
       </c>
       <c r="B84" t="s">
-        <v>284</v>
+        <v>147</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -2312,21 +2343,21 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>41</v>
+        <v>283</v>
       </c>
       <c r="B85" t="s">
-        <v>42</v>
+        <v>284</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B86" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C86">
         <v>2</v>
@@ -2334,10 +2365,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B87" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C87">
         <v>2</v>
@@ -2345,10 +2376,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B88" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C88">
         <v>2</v>
@@ -2356,10 +2387,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B89" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C89">
         <v>2</v>
@@ -2367,10 +2398,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B90" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C90">
         <v>2</v>
@@ -2378,10 +2409,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B91" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C91">
         <v>2</v>
@@ -2389,10 +2420,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>285</v>
+        <v>53</v>
       </c>
       <c r="B92" t="s">
-        <v>286</v>
+        <v>54</v>
       </c>
       <c r="C92">
         <v>2</v>
@@ -2400,10 +2431,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>55</v>
+        <v>285</v>
       </c>
       <c r="B93" t="s">
-        <v>56</v>
+        <v>286</v>
       </c>
       <c r="C93">
         <v>2</v>
@@ -2411,10 +2442,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B94" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C94">
         <v>2</v>
@@ -2422,21 +2453,21 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>287</v>
+        <v>57</v>
       </c>
       <c r="B95" t="s">
-        <v>288</v>
+        <v>58</v>
       </c>
       <c r="C95">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>148</v>
+        <v>287</v>
       </c>
       <c r="B96" t="s">
-        <v>149</v>
+        <v>288</v>
       </c>
       <c r="C96">
         <v>3</v>
@@ -2444,65 +2475,65 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>289</v>
+        <v>148</v>
       </c>
       <c r="B97" t="s">
-        <v>290</v>
+        <v>149</v>
       </c>
       <c r="C97">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>150</v>
+        <v>289</v>
       </c>
       <c r="B98" t="s">
-        <v>151</v>
+        <v>290</v>
       </c>
       <c r="C98">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="B99" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>291</v>
+        <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>292</v>
+        <v>17</v>
       </c>
       <c r="C100">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B101" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C101">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>152</v>
+        <v>293</v>
       </c>
       <c r="B102" t="s">
-        <v>153</v>
+        <v>294</v>
       </c>
       <c r="C102">
         <v>3</v>
@@ -2510,29 +2541,32 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
       <c r="B103" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="C103">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>295</v>
+        <v>59</v>
       </c>
       <c r="B104" t="s">
-        <v>296</v>
+        <v>60</v>
       </c>
       <c r="C104">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>297</v>
+        <v>295</v>
+      </c>
+      <c r="B105" t="s">
+        <v>296</v>
       </c>
       <c r="C105">
         <v>3</v>
@@ -2661,21 +2695,21 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="B117" t="s">
-        <v>300</v>
+        <v>324</v>
       </c>
       <c r="C117">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>167</v>
+        <v>299</v>
       </c>
       <c r="B118" t="s">
-        <v>168</v>
+        <v>300</v>
       </c>
       <c r="C118">
         <v>3</v>
@@ -2683,10 +2717,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B119" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C119">
         <v>3</v>
@@ -2694,54 +2728,54 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="B120" t="s">
-        <v>234</v>
+        <v>170</v>
       </c>
       <c r="C120">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>301</v>
+        <v>233</v>
       </c>
       <c r="B121" t="s">
-        <v>302</v>
+        <v>234</v>
       </c>
       <c r="C121">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>18</v>
+        <v>301</v>
       </c>
       <c r="B122" t="s">
-        <v>19</v>
+        <v>302</v>
       </c>
       <c r="C122">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="B123" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="C123">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>303</v>
+        <v>63</v>
       </c>
       <c r="B124" t="s">
-        <v>304</v>
+        <v>64</v>
       </c>
       <c r="C124">
         <v>2</v>
@@ -2749,10 +2783,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>65</v>
+        <v>303</v>
       </c>
       <c r="B125" t="s">
-        <v>66</v>
+        <v>304</v>
       </c>
       <c r="C125">
         <v>2</v>
@@ -2760,21 +2794,21 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>171</v>
+        <v>65</v>
       </c>
       <c r="B126" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
       <c r="C126">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B127" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C127">
         <v>3</v>
@@ -2782,10 +2816,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B128" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C128">
         <v>3</v>
@@ -2793,10 +2827,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B129" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C129">
         <v>3</v>
@@ -2804,10 +2838,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B130" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C130">
         <v>3</v>
@@ -2815,10 +2849,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B131" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C131">
         <v>3</v>
@@ -2826,10 +2860,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B132" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C132">
         <v>3</v>
@@ -2837,10 +2871,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>305</v>
+        <v>183</v>
       </c>
       <c r="B133" t="s">
-        <v>306</v>
+        <v>184</v>
       </c>
       <c r="C133">
         <v>3</v>
@@ -2848,10 +2882,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>185</v>
+        <v>305</v>
       </c>
       <c r="B134" t="s">
-        <v>186</v>
+        <v>306</v>
       </c>
       <c r="C134">
         <v>3</v>
@@ -2859,21 +2893,21 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>67</v>
+        <v>185</v>
       </c>
       <c r="B135" t="s">
-        <v>68</v>
+        <v>186</v>
       </c>
       <c r="C135">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B136" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C136">
         <v>2</v>
@@ -2881,10 +2915,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B137" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C137">
         <v>2</v>
@@ -2892,21 +2926,21 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>187</v>
+        <v>71</v>
       </c>
       <c r="B138" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="C138">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B139" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C139">
         <v>3</v>
@@ -2914,10 +2948,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B140" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C140">
         <v>3</v>
@@ -2925,10 +2959,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B141" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C141">
         <v>3</v>
@@ -2936,7 +2970,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>316</v>
+        <v>193</v>
+      </c>
+      <c r="B142" t="s">
+        <v>194</v>
       </c>
       <c r="C142">
         <v>3</v>
@@ -2944,10 +2981,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>195</v>
+        <v>316</v>
       </c>
       <c r="B143" t="s">
-        <v>196</v>
+        <v>323</v>
       </c>
       <c r="C143">
         <v>3</v>
@@ -2955,10 +2992,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C144">
         <v>3</v>
@@ -2966,10 +3003,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B145" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C145">
         <v>3</v>
@@ -2977,10 +3014,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B146" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C146">
         <v>3</v>
@@ -2988,10 +3025,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>307</v>
+        <v>201</v>
       </c>
       <c r="B147" t="s">
-        <v>308</v>
+        <v>202</v>
       </c>
       <c r="C147">
         <v>3</v>
@@ -2999,32 +3036,32 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>73</v>
+        <v>307</v>
       </c>
       <c r="B148" t="s">
-        <v>74</v>
+        <v>308</v>
       </c>
       <c r="C148">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>203</v>
+        <v>73</v>
       </c>
       <c r="B149" t="s">
-        <v>204</v>
+        <v>74</v>
       </c>
       <c r="C149">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B150" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C150">
         <v>3</v>
@@ -3032,32 +3069,32 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>20</v>
+        <v>205</v>
       </c>
       <c r="B151" t="s">
-        <v>21</v>
+        <v>206</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="C152">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B153" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C153">
         <v>2</v>
@@ -3065,21 +3102,21 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>207</v>
+        <v>77</v>
       </c>
       <c r="B154" t="s">
-        <v>208</v>
+        <v>78</v>
       </c>
       <c r="C154">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B155" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C155">
         <v>3</v>
@@ -3087,10 +3124,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B156" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C156">
         <v>3</v>
@@ -3098,21 +3135,21 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>79</v>
+        <v>211</v>
       </c>
       <c r="B157" t="s">
-        <v>80</v>
+        <v>212</v>
       </c>
       <c r="C157">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B158" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C158">
         <v>2</v>
@@ -3120,21 +3157,21 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>213</v>
+        <v>81</v>
       </c>
       <c r="B159" t="s">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="C159">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B160" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C160">
         <v>3</v>
@@ -3142,32 +3179,35 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>83</v>
+        <v>215</v>
       </c>
       <c r="B161" t="s">
-        <v>84</v>
+        <v>216</v>
       </c>
       <c r="C161">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>217</v>
+        <v>83</v>
       </c>
       <c r="B162" t="s">
-        <v>218</v>
+        <v>84</v>
       </c>
       <c r="C162">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>318</v>
+        <v>217</v>
+      </c>
+      <c r="B163" t="s">
+        <v>218</v>
       </c>
       <c r="C163">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>